<commit_message>
Added to levels and stats spreadsheet
</commit_message>
<xml_diff>
--- a/Game Files/Levels and Stats.xlsx
+++ b/Game Files/Levels and Stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akswa\Documents\Godot\Projects\Roguelike DnDish\Game Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2454A9E4-5A5B-4778-B7ED-6F6DE9896ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F29E78F-ADC2-4031-BB11-62F0438735E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33240" yWindow="2685" windowWidth="21600" windowHeight="11295" xr2:uid="{6B97E4FA-83C8-4540-8556-46C465D5AB8C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6B97E4FA-83C8-4540-8556-46C465D5AB8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="60">
   <si>
     <t>Level</t>
   </si>
@@ -189,6 +189,33 @@
   </si>
   <si>
     <t>Side Wall(1 Floor)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      </t>
+  </si>
+  <si>
+    <t>Rat</t>
+  </si>
+  <si>
+    <t>Floor Timer</t>
+  </si>
+  <si>
+    <t>Increase difficulty with time</t>
+  </si>
+  <si>
+    <t>Mobs</t>
+  </si>
+  <si>
+    <t>Build</t>
+  </si>
+  <si>
+    <t>Up</t>
+  </si>
+  <si>
+    <t>Portal</t>
+  </si>
+  <si>
+    <t>Village</t>
   </si>
 </sst>
 </file>
@@ -224,7 +251,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -321,6 +348,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="45">
     <border>
@@ -889,7 +934,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1049,28 +1094,28 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1079,29 +1124,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1109,17 +1136,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1172,6 +1226,223 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F32CA4C-D6C4-4158-58D6-3F0EB13D250C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8467725" y="9163050"/>
+          <a:ext cx="1533525" cy="19050"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1009650</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38ACB129-E1E5-071A-74A5-C97539AA22B5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9944100" y="8248650"/>
+          <a:ext cx="323850" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA7D3160-2141-80E9-5F1F-0594D5728D0D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="12496800" y="8334375"/>
+          <a:ext cx="352425" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1592F37B-5EA9-3755-F3AC-E30A80F9CBB5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="12715875" y="9477375"/>
+          <a:ext cx="2238375" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1493,8 +1764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26B65FB3-4F24-4A40-A91F-52687A3EE8E7}">
   <dimension ref="A1:W67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1556,11 +1827,11 @@
         <v>9</v>
       </c>
       <c r="R2" s="53"/>
-      <c r="S2" s="67" t="s">
+      <c r="S2" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="T2" s="68"/>
-      <c r="U2" s="68"/>
+      <c r="T2" s="84"/>
+      <c r="U2" s="84"/>
       <c r="V2" s="58"/>
     </row>
     <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1639,11 +1910,11 @@
         <v>4</v>
       </c>
       <c r="R4" s="54"/>
-      <c r="S4" s="61" t="s">
+      <c r="S4" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="T4" s="62"/>
-      <c r="U4" s="63"/>
+      <c r="T4" s="78"/>
+      <c r="U4" s="79"/>
       <c r="V4" s="59"/>
       <c r="W4" s="14" t="s">
         <v>29</v>
@@ -1686,11 +1957,11 @@
         <v>4</v>
       </c>
       <c r="R5" s="54"/>
-      <c r="S5" s="64" t="s">
+      <c r="S5" s="80" t="s">
         <v>35</v>
       </c>
-      <c r="T5" s="65"/>
-      <c r="U5" s="66"/>
+      <c r="T5" s="81"/>
+      <c r="U5" s="82"/>
       <c r="V5" s="59"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
@@ -2166,11 +2437,11 @@
         <v>0.8</v>
       </c>
       <c r="R15" s="54"/>
-      <c r="S15" s="61" t="s">
+      <c r="S15" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="T15" s="62"/>
-      <c r="U15" s="63"/>
+      <c r="T15" s="78"/>
+      <c r="U15" s="79"/>
       <c r="V15" s="59"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
@@ -2211,11 +2482,11 @@
         <v>1.2</v>
       </c>
       <c r="R16" s="54"/>
-      <c r="S16" s="64" t="s">
+      <c r="S16" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="T16" s="65"/>
-      <c r="U16" s="66"/>
+      <c r="T16" s="81"/>
+      <c r="U16" s="82"/>
       <c r="V16" s="59"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
@@ -2469,14 +2740,14 @@
         <f t="shared" si="2"/>
         <v>28421.709430404007</v>
       </c>
-      <c r="K22" s="77" t="s">
+      <c r="K22" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="L22" s="78"/>
-      <c r="M22" s="75" t="s">
+      <c r="L22" s="76"/>
+      <c r="M22" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="N22" s="76" t="s">
+      <c r="N22" s="66" t="s">
         <v>46</v>
       </c>
       <c r="R22" s="54"/>
@@ -2509,14 +2780,14 @@
         <f t="shared" si="2"/>
         <v>35527.136788005009</v>
       </c>
-      <c r="K23" s="79" t="s">
+      <c r="K23" s="73" t="s">
         <v>47</v>
       </c>
-      <c r="L23" s="80"/>
-      <c r="M23" s="73">
+      <c r="L23" s="74"/>
+      <c r="M23" s="63">
         <v>100</v>
       </c>
-      <c r="N23" s="74">
+      <c r="N23" s="64">
         <v>76</v>
       </c>
       <c r="R23" s="54"/>
@@ -2549,15 +2820,15 @@
         <f t="shared" si="2"/>
         <v>44408.920985006262</v>
       </c>
-      <c r="K24" s="81" t="s">
+      <c r="K24" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="L24" s="82"/>
-      <c r="M24" s="71">
+      <c r="L24" s="72"/>
+      <c r="M24" s="61">
         <f>M23*1.25</f>
         <v>125</v>
       </c>
-      <c r="N24" s="72">
+      <c r="N24" s="62">
         <f>86</f>
         <v>86</v>
       </c>
@@ -2591,16 +2862,19 @@
         <f t="shared" si="2"/>
         <v>55511.151231257827</v>
       </c>
-      <c r="K25" s="81" t="s">
+      <c r="J25" t="s">
+        <v>29</v>
+      </c>
+      <c r="K25" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="L25" s="82"/>
-      <c r="M25" s="71">
+      <c r="L25" s="72"/>
+      <c r="M25" s="61">
         <f>M23*1.4</f>
         <v>140</v>
       </c>
-      <c r="N25" s="72">
-        <v>86</v>
+      <c r="N25" s="62" t="s">
+        <v>51</v>
       </c>
       <c r="R25" s="55"/>
       <c r="S25" s="56"/>
@@ -2628,13 +2902,10 @@
         <v>50</v>
       </c>
       <c r="L26" s="70"/>
-      <c r="M26" s="83">
+      <c r="M26" s="67">
         <v>140</v>
       </c>
-      <c r="N26" s="84">
-        <f>N25/2</f>
-        <v>43</v>
-      </c>
+      <c r="N26" s="68"/>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27">
@@ -2698,6 +2969,10 @@
       <c r="N29" s="17" t="s">
         <v>26</v>
       </c>
+      <c r="O29" s="85">
+        <f>N30/M33</f>
+        <v>35.880398671096344</v>
+      </c>
     </row>
     <row r="30" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30">
@@ -2716,18 +2991,22 @@
         <v>169406.58945086005</v>
       </c>
       <c r="K30" s="18">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="L30" s="19">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="M30" s="20">
         <f>IF(K30=L30,IF(ABS(K30-L30)&gt;3,3,IF(L30&gt;0,ABS(K30/L30),3)),0.55+(IF(ABS(K30-L30)&gt;3,3,IF(L30&gt;0,ABS(K30/L30),3))/2))</f>
-        <v>1</v>
+        <v>0.71666666666666667</v>
       </c>
       <c r="N30" s="21">
         <f>VLOOKUP(L30,A1:B52,2,FALSE)</f>
-        <v>10000</v>
+        <v>900</v>
+      </c>
+      <c r="O30">
+        <f>400/28</f>
+        <v>14.285714285714286</v>
       </c>
     </row>
     <row r="31" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2770,7 +3049,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -2791,10 +3070,19 @@
       </c>
       <c r="M33" s="25">
         <f>(25+(0.1*VLOOKUP(K30,A2:B52,2,FALSE)*1))*M30</f>
-        <v>1025</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+        <v>25.083333333333332</v>
+      </c>
+      <c r="O33" t="s">
+        <v>52</v>
+      </c>
+      <c r="P33">
+        <v>1</v>
+      </c>
+      <c r="Q33">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -2815,10 +3103,16 @@
       </c>
       <c r="M34" s="26">
         <f>M33*1.5</f>
-        <v>1537.5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>37.625</v>
+      </c>
+      <c r="P34">
+        <v>2</v>
+      </c>
+      <c r="Q34">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2839,15 +3133,21 @@
       </c>
       <c r="M35" s="27">
         <f>M33*2</f>
-        <v>2050</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+        <v>50.166666666666664</v>
+      </c>
+      <c r="P35">
+        <v>3</v>
+      </c>
+      <c r="Q35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36" s="1">
-        <f t="shared" ref="B36:B67" si="5">$B$3*(A36^2)</f>
+        <f t="shared" ref="B36:B52" si="5">$B$3*(A36^2)</f>
         <v>115600</v>
       </c>
       <c r="C36" s="1">
@@ -2859,7 +3159,7 @@
         <v>646234.85355705279</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2876,7 +3176,7 @@
         <v>807793.56694631604</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -2892,8 +3192,14 @@
         <f t="shared" si="2"/>
         <v>1009741.9586828951</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L38" s="86" t="s">
+        <v>53</v>
+      </c>
+      <c r="M38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2909,8 +3215,14 @@
         <f t="shared" si="2"/>
         <v>1262177.4483536188</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L39" s="87" t="s">
+        <v>58</v>
+      </c>
+      <c r="O39" s="87" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -2926,8 +3238,14 @@
         <f t="shared" si="2"/>
         <v>1577721.8104420234</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L40" s="88" t="s">
+        <v>55</v>
+      </c>
+      <c r="O40" s="88" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2943,8 +3261,14 @@
         <f t="shared" si="2"/>
         <v>1972152.2630525292</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L41" s="88" t="s">
+        <v>56</v>
+      </c>
+      <c r="O41" s="88" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2960,8 +3284,14 @@
         <f t="shared" si="2"/>
         <v>2465190.3288156614</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L42" s="88" t="s">
+        <v>57</v>
+      </c>
+      <c r="O42" s="88" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2978,7 +3308,7 @@
         <v>3081487.9110195767</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2995,7 +3325,7 @@
         <v>3851859.8887744709</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -3012,7 +3342,7 @@
         <v>4814824.8609680887</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -3028,8 +3358,12 @@
         <f t="shared" si="2"/>
         <v>6018531.0762101114</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M46" s="89" t="s">
+        <v>59</v>
+      </c>
+      <c r="N46" s="89"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -3045,8 +3379,16 @@
         <f t="shared" si="2"/>
         <v>7523163.8452626392</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J47" s="87" t="s">
+        <v>58</v>
+      </c>
+      <c r="M47" s="89"/>
+      <c r="N47" s="89"/>
+      <c r="R47" s="87" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -3062,8 +3404,16 @@
         <f t="shared" si="2"/>
         <v>9403954.806578299</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J48" s="88" t="s">
+        <v>55</v>
+      </c>
+      <c r="M48" s="89"/>
+      <c r="N48" s="89"/>
+      <c r="R48" s="88" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -3079,8 +3429,16 @@
         <f t="shared" si="2"/>
         <v>11754943.508222874</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J49" s="88" t="s">
+        <v>56</v>
+      </c>
+      <c r="M49" s="89"/>
+      <c r="N49" s="89"/>
+      <c r="R49" s="88" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
@@ -3096,8 +3454,16 @@
         <f t="shared" si="2"/>
         <v>14693679.385278594</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J50" s="88" t="s">
+        <v>57</v>
+      </c>
+      <c r="M50" s="89"/>
+      <c r="N50" s="89"/>
+      <c r="R50" s="88" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -3114,7 +3480,7 @@
         <v>18367099.231598243</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
@@ -3130,8 +3496,14 @@
         <f t="shared" si="2"/>
         <v>22958874.039497804</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="M52" s="88" t="s">
+        <v>22</v>
+      </c>
+      <c r="N52" s="88" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
@@ -3148,7 +3520,7 @@
         <v>28698592.549372256</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
@@ -3165,7 +3537,7 @@
         <v>35873240.68671532</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
@@ -3182,7 +3554,7 @@
         <v>44841550.858394146</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
@@ -3199,7 +3571,7 @@
         <v>56051938.572992682</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -3216,7 +3588,7 @@
         <v>70064923.216240853</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
@@ -3233,7 +3605,7 @@
         <v>87581154.020301074</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
@@ -3250,7 +3622,7 @@
         <v>109476442.52537635</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
@@ -3267,7 +3639,7 @@
         <v>136845553.15672043</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
@@ -3284,7 +3656,7 @@
         <v>171056941.44590053</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
@@ -3301,7 +3673,7 @@
         <v>213821176.80737567</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
@@ -3318,7 +3690,7 @@
         <v>267276471.00921959</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
@@ -3387,17 +3759,18 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="M46:N50"/>
+    <mergeCell ref="S15:U15"/>
+    <mergeCell ref="S16:U16"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="S2:U2"/>
     <mergeCell ref="K26:L26"/>
     <mergeCell ref="K24:L24"/>
     <mergeCell ref="K23:L23"/>
     <mergeCell ref="K25:L25"/>
     <mergeCell ref="K22:L22"/>
-    <mergeCell ref="S15:U15"/>
-    <mergeCell ref="S16:U16"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="S2:U2"/>
   </mergeCells>
   <conditionalFormatting sqref="K10:P10">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
@@ -3416,5 +3789,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
reimported assets for base human. Changed godot rendering settings to linear mipmap
</commit_message>
<xml_diff>
--- a/Game Files/Levels and Stats.xlsx
+++ b/Game Files/Levels and Stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akswa\Documents\Godot\Projects\Roguelike DnDish\Game Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F29E78F-ADC2-4031-BB11-62F0438735E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EED6D1A-F56D-4349-A61C-3FA21A601DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6B97E4FA-83C8-4540-8556-46C465D5AB8C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="61">
   <si>
     <t>Level</t>
   </si>
@@ -216,6 +216,9 @@
   </si>
   <si>
     <t>Village</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        </t>
   </si>
 </sst>
 </file>
@@ -1118,62 +1121,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1764,8 +1767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26B65FB3-4F24-4A40-A91F-52687A3EE8E7}">
   <dimension ref="A1:W67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="M46" sqref="M46:N50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1827,11 +1830,11 @@
         <v>9</v>
       </c>
       <c r="R2" s="53"/>
-      <c r="S2" s="83" t="s">
+      <c r="S2" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="T2" s="84"/>
-      <c r="U2" s="84"/>
+      <c r="T2" s="81"/>
+      <c r="U2" s="81"/>
       <c r="V2" s="58"/>
     </row>
     <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1910,11 +1913,11 @@
         <v>4</v>
       </c>
       <c r="R4" s="54"/>
-      <c r="S4" s="77" t="s">
+      <c r="S4" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="T4" s="78"/>
-      <c r="U4" s="79"/>
+      <c r="T4" s="75"/>
+      <c r="U4" s="76"/>
       <c r="V4" s="59"/>
       <c r="W4" s="14" t="s">
         <v>29</v>
@@ -1957,11 +1960,11 @@
         <v>4</v>
       </c>
       <c r="R5" s="54"/>
-      <c r="S5" s="80" t="s">
+      <c r="S5" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="T5" s="81"/>
-      <c r="U5" s="82"/>
+      <c r="T5" s="78"/>
+      <c r="U5" s="79"/>
       <c r="V5" s="59"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
@@ -2437,11 +2440,11 @@
         <v>0.8</v>
       </c>
       <c r="R15" s="54"/>
-      <c r="S15" s="77" t="s">
+      <c r="S15" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="T15" s="78"/>
-      <c r="U15" s="79"/>
+      <c r="T15" s="75"/>
+      <c r="U15" s="76"/>
       <c r="V15" s="59"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
@@ -2482,11 +2485,11 @@
         <v>1.2</v>
       </c>
       <c r="R16" s="54"/>
-      <c r="S16" s="80" t="s">
+      <c r="S16" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="T16" s="81"/>
-      <c r="U16" s="82"/>
+      <c r="T16" s="78"/>
+      <c r="U16" s="79"/>
       <c r="V16" s="59"/>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
@@ -2740,10 +2743,10 @@
         <f t="shared" si="2"/>
         <v>28421.709430404007</v>
       </c>
-      <c r="K22" s="75" t="s">
+      <c r="K22" s="88" t="s">
         <v>48</v>
       </c>
-      <c r="L22" s="76"/>
+      <c r="L22" s="89"/>
       <c r="M22" s="65" t="s">
         <v>45</v>
       </c>
@@ -2780,10 +2783,10 @@
         <f t="shared" si="2"/>
         <v>35527.136788005009</v>
       </c>
-      <c r="K23" s="73" t="s">
+      <c r="K23" s="86" t="s">
         <v>47</v>
       </c>
-      <c r="L23" s="74"/>
+      <c r="L23" s="87"/>
       <c r="M23" s="63">
         <v>100</v>
       </c>
@@ -2820,10 +2823,10 @@
         <f t="shared" si="2"/>
         <v>44408.920985006262</v>
       </c>
-      <c r="K24" s="71" t="s">
+      <c r="K24" s="84" t="s">
         <v>44</v>
       </c>
-      <c r="L24" s="72"/>
+      <c r="L24" s="85"/>
       <c r="M24" s="61">
         <f>M23*1.25</f>
         <v>125</v>
@@ -2865,13 +2868,12 @@
       <c r="J25" t="s">
         <v>29</v>
       </c>
-      <c r="K25" s="71" t="s">
+      <c r="K25" s="84" t="s">
         <v>49</v>
       </c>
-      <c r="L25" s="72"/>
-      <c r="M25" s="61">
-        <f>M23*1.4</f>
-        <v>140</v>
+      <c r="L25" s="85"/>
+      <c r="M25" s="61" t="s">
+        <v>60</v>
       </c>
       <c r="N25" s="62" t="s">
         <v>51</v>
@@ -2898,10 +2900,10 @@
         <f t="shared" si="2"/>
         <v>69388.939039072284</v>
       </c>
-      <c r="K26" s="69" t="s">
+      <c r="K26" s="82" t="s">
         <v>50</v>
       </c>
-      <c r="L26" s="70"/>
+      <c r="L26" s="83"/>
       <c r="M26" s="67">
         <v>140</v>
       </c>
@@ -2969,7 +2971,7 @@
       <c r="N29" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="O29" s="85">
+      <c r="O29" s="69">
         <f>N30/M33</f>
         <v>35.880398671096344</v>
       </c>
@@ -3175,6 +3177,9 @@
         <f t="shared" si="2"/>
         <v>807793.56694631604</v>
       </c>
+      <c r="H37" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38">
@@ -3192,7 +3197,7 @@
         <f t="shared" si="2"/>
         <v>1009741.9586828951</v>
       </c>
-      <c r="L38" s="86" t="s">
+      <c r="L38" s="70" t="s">
         <v>53</v>
       </c>
       <c r="M38" t="s">
@@ -3215,10 +3220,10 @@
         <f t="shared" si="2"/>
         <v>1262177.4483536188</v>
       </c>
-      <c r="L39" s="87" t="s">
+      <c r="L39" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="O39" s="87" t="s">
+      <c r="O39" s="71" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3238,10 +3243,10 @@
         <f t="shared" si="2"/>
         <v>1577721.8104420234</v>
       </c>
-      <c r="L40" s="88" t="s">
+      <c r="L40" s="72" t="s">
         <v>55</v>
       </c>
-      <c r="O40" s="88" t="s">
+      <c r="O40" s="72" t="s">
         <v>55</v>
       </c>
     </row>
@@ -3261,10 +3266,10 @@
         <f t="shared" si="2"/>
         <v>1972152.2630525292</v>
       </c>
-      <c r="L41" s="88" t="s">
+      <c r="L41" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="O41" s="88" t="s">
+      <c r="O41" s="72" t="s">
         <v>56</v>
       </c>
     </row>
@@ -3284,10 +3289,10 @@
         <f t="shared" si="2"/>
         <v>2465190.3288156614</v>
       </c>
-      <c r="L42" s="88" t="s">
+      <c r="L42" s="72" t="s">
         <v>57</v>
       </c>
-      <c r="O42" s="88" t="s">
+      <c r="O42" s="72" t="s">
         <v>57</v>
       </c>
     </row>
@@ -3358,10 +3363,10 @@
         <f t="shared" si="2"/>
         <v>6018531.0762101114</v>
       </c>
-      <c r="M46" s="89" t="s">
+      <c r="M46" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="N46" s="89"/>
+      <c r="N46" s="73"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47">
@@ -3379,12 +3384,12 @@
         <f t="shared" si="2"/>
         <v>7523163.8452626392</v>
       </c>
-      <c r="J47" s="87" t="s">
+      <c r="J47" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="M47" s="89"/>
-      <c r="N47" s="89"/>
-      <c r="R47" s="87" t="s">
+      <c r="M47" s="73"/>
+      <c r="N47" s="73"/>
+      <c r="R47" s="71" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3404,12 +3409,12 @@
         <f t="shared" si="2"/>
         <v>9403954.806578299</v>
       </c>
-      <c r="J48" s="88" t="s">
+      <c r="J48" s="72" t="s">
         <v>55</v>
       </c>
-      <c r="M48" s="89"/>
-      <c r="N48" s="89"/>
-      <c r="R48" s="88" t="s">
+      <c r="M48" s="73"/>
+      <c r="N48" s="73"/>
+      <c r="R48" s="72" t="s">
         <v>55</v>
       </c>
     </row>
@@ -3429,12 +3434,12 @@
         <f t="shared" si="2"/>
         <v>11754943.508222874</v>
       </c>
-      <c r="J49" s="88" t="s">
+      <c r="J49" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="M49" s="89"/>
-      <c r="N49" s="89"/>
-      <c r="R49" s="88" t="s">
+      <c r="M49" s="73"/>
+      <c r="N49" s="73"/>
+      <c r="R49" s="72" t="s">
         <v>56</v>
       </c>
     </row>
@@ -3454,12 +3459,15 @@
         <f t="shared" si="2"/>
         <v>14693679.385278594</v>
       </c>
-      <c r="J50" s="88" t="s">
+      <c r="J50" s="72" t="s">
         <v>57</v>
       </c>
-      <c r="M50" s="89"/>
-      <c r="N50" s="89"/>
-      <c r="R50" s="88" t="s">
+      <c r="M50" s="73"/>
+      <c r="N50" s="73"/>
+      <c r="O50" t="s">
+        <v>29</v>
+      </c>
+      <c r="R50" s="72" t="s">
         <v>57</v>
       </c>
     </row>
@@ -3496,10 +3504,10 @@
         <f t="shared" si="2"/>
         <v>22958874.039497804</v>
       </c>
-      <c r="M52" s="88" t="s">
+      <c r="M52" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="N52" s="88" t="s">
+      <c r="N52" s="72" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3760,17 +3768,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="M46:N50"/>
-    <mergeCell ref="S15:U15"/>
-    <mergeCell ref="S16:U16"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="S5:U5"/>
     <mergeCell ref="S2:U2"/>
     <mergeCell ref="K26:L26"/>
     <mergeCell ref="K24:L24"/>
     <mergeCell ref="K23:L23"/>
     <mergeCell ref="K25:L25"/>
     <mergeCell ref="K22:L22"/>
+    <mergeCell ref="M46:N50"/>
+    <mergeCell ref="S15:U15"/>
+    <mergeCell ref="S16:U16"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="S5:U5"/>
   </mergeCells>
   <conditionalFormatting sqref="K10:P10">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">

</xml_diff>